<commit_message>
labs: finalise lab 02
</commit_message>
<xml_diff>
--- a/labs/data/soil.xlsx
+++ b/labs/data/soil.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fvanogtrop\Dropbox (Sydney Uni)\TEACHING\ENVX\ENVX2020\ENVX1002\Module_1_Data\2020\Practical\Topic 2\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhar8696/Documents/ENVX1002-handbook/labs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30DDC48F-620E-4DA3-9FCE-CB2A820B88A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42AB8ED-54D2-0048-950F-60C9D1BA3161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SO4" sheetId="13" r:id="rId1"/>
     <sheet name="soil" sheetId="14" r:id="rId2"/>
+    <sheet name="SO4_excel" sheetId="15" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="genes">#REF!</definedName>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="71">
   <si>
     <t>SO4</t>
   </si>
@@ -296,24 +297,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -338,9 +338,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -378,9 +378,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -413,26 +413,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -465,26 +448,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -664,14 +630,14 @@
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="3" width="8.85546875" style="2"/>
-    <col min="4" max="4" width="21.85546875" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="3" width="8.83203125" style="2"/>
+    <col min="4" max="4" width="21.83203125" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -679,255 +645,255 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A2" s="2">
         <v>50.6</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" s="2">
         <v>55.4</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" s="2">
         <v>56.5</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" s="2">
         <v>57.5</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+      <c r="D5" s="7"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" s="2">
         <v>58.3</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+      <c r="D6" s="7"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7" s="2">
         <v>63</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
+      <c r="D7" s="7"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A8" s="2">
         <v>66.5</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A9" s="2">
         <v>64.5</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A10" s="2">
         <v>63.4</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A11" s="2">
         <v>58.4</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A12" s="2">
         <v>70.599999999999994</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="7"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A13" s="2">
         <v>56.9</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="8"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="7"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14" s="2">
         <v>56.7</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="8"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="7"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A15" s="2">
         <v>56</v>
       </c>
-      <c r="E15" s="8"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A16" s="2">
         <v>60.4</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
+      <c r="D16" s="7"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A17" s="2">
         <v>67.8</v>
       </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
+      <c r="D17" s="7"/>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A18" s="2">
         <v>70.8</v>
       </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
+      <c r="D18" s="8"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A19" s="2">
         <v>58.6</v>
       </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A20" s="2">
         <v>59.5</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="3">
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A21" s="2">
         <v>55.5</v>
       </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="3">
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A22" s="2">
         <v>63.4</v>
       </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="3">
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A23" s="2">
         <v>57.8</v>
       </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="3">
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A24" s="2">
         <v>55.1</v>
       </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="3">
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A25" s="2">
         <v>65.5</v>
       </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="3">
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A26" s="2">
         <v>62.7</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A27" s="2">
         <v>72.099999999999994</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A28" s="2">
         <v>63.4</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A29" s="2">
         <v>68.5</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A30" s="2">
         <v>65.8</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A31" s="2">
         <v>69.2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A32" s="2">
         <v>66.7</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A33" s="2">
         <v>59.3</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A34" s="2">
         <v>61.1</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A35" s="2">
         <v>62.1</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A36" s="2">
         <v>70.400000000000006</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A37" s="2">
         <v>62.1</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A38" s="2">
         <v>64.599999999999994</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A39" s="2">
         <v>61.4</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A40" s="2">
         <v>56.9</v>
       </c>
     </row>
@@ -947,13 +913,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -976,7 +942,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -999,7 +965,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1022,7 +988,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1045,7 +1011,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1068,7 +1034,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1091,7 +1057,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1114,7 +1080,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1137,7 +1103,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1160,7 +1126,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1183,7 +1149,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1206,7 +1172,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1229,7 +1195,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1252,7 +1218,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1275,7 +1241,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1298,7 +1264,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1321,7 +1287,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -1344,7 +1310,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1367,7 +1333,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1390,7 +1356,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -1413,7 +1379,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -1436,7 +1402,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -1459,7 +1425,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -1482,7 +1448,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -1505,7 +1471,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -1528,7 +1494,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -1551,7 +1517,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -1574,7 +1540,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -1597,7 +1563,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -1620,7 +1586,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -1643,7 +1609,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -1666,7 +1632,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>44</v>
       </c>
@@ -1689,7 +1655,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>45</v>
       </c>
@@ -1712,7 +1678,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>46</v>
       </c>
@@ -1735,7 +1701,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>47</v>
       </c>
@@ -1758,7 +1724,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>48</v>
       </c>
@@ -1781,7 +1747,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>49</v>
       </c>
@@ -1804,7 +1770,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>50</v>
       </c>
@@ -1827,7 +1793,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>51</v>
       </c>
@@ -1850,7 +1816,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>53</v>
       </c>
@@ -1873,7 +1839,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>54</v>
       </c>
@@ -1896,7 +1862,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>55</v>
       </c>
@@ -1919,7 +1885,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>56</v>
       </c>
@@ -1936,7 +1902,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
         <v>57</v>
       </c>
@@ -1959,7 +1925,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
         <v>58</v>
       </c>
@@ -1982,7 +1948,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
         <v>59</v>
       </c>
@@ -2005,7 +1971,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
         <v>60</v>
       </c>
@@ -2028,7 +1994,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
         <v>61</v>
       </c>
@@ -2051,7 +2017,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
         <v>62</v>
       </c>
@@ -2074,7 +2040,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
         <v>63</v>
       </c>
@@ -2097,7 +2063,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
         <v>64</v>
       </c>
@@ -2120,7 +2086,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
         <v>65</v>
       </c>
@@ -2143,7 +2109,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
         <v>67</v>
       </c>
@@ -2166,7 +2132,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
         <v>68</v>
       </c>
@@ -2189,7 +2155,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
         <v>69</v>
       </c>
@@ -2212,7 +2178,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
         <v>70</v>
       </c>
@@ -2243,4 +2209,284 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4465FFB1-ECE7-5B40-BCA3-1DD91254EEA6}">
+  <dimension ref="A1:E40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="3" width="8.83203125" style="2"/>
+    <col min="4" max="4" width="21.83203125" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A2" s="2">
+        <v>50.6</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" s="2">
+        <v>55.4</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" s="2">
+        <v>56.5</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" s="2">
+        <v>57.5</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" s="2">
+        <v>58.3</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7" s="2">
+        <v>63</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A8" s="2">
+        <v>66.5</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A9" s="2">
+        <v>64.5</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A10" s="2">
+        <v>63.4</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A11" s="2">
+        <v>58.4</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A12" s="2">
+        <v>70.599999999999994</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A13" s="2">
+        <v>56.9</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="7"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14" s="2">
+        <v>56.7</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="7"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A15" s="2">
+        <v>56</v>
+      </c>
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A16" s="2">
+        <v>60.4</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A17" s="2">
+        <v>67.8</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A18" s="2">
+        <v>70.8</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A19" s="2">
+        <v>58.6</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A20" s="2">
+        <v>59.5</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A21" s="2">
+        <v>55.5</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A22" s="2">
+        <v>63.4</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A23" s="2">
+        <v>57.8</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A24" s="2">
+        <v>55.1</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A25" s="2">
+        <v>65.5</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A26" s="2">
+        <v>62.7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A27" s="2">
+        <v>72.099999999999994</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A28" s="2">
+        <v>63.4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A29" s="2">
+        <v>68.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A30" s="2">
+        <v>65.8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A31" s="2">
+        <v>69.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A32" s="2">
+        <v>66.7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A33" s="2">
+        <v>59.3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A34" s="2">
+        <v>61.1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A35" s="2">
+        <v>62.1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A36" s="2">
+        <v>70.400000000000006</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A37" s="2">
+        <v>62.1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A38" s="2">
+        <v>64.599999999999994</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A39" s="2">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A40" s="2">
+        <v>56.9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
 </file>
</xml_diff>